<commit_message>
:+1: Done salary managerment
</commit_message>
<xml_diff>
--- a/api/src/template/salary_template.xlsx
+++ b/api/src/template/salary_template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Salary" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Salary!$A$6:$P$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Salary!$A$6:$Q$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>No</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Back account</t>
+  </si>
+  <si>
+    <t>Bonus reward</t>
   </si>
 </sst>
 </file>
@@ -170,6 +173,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -178,12 +187,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -484,157 +487,165 @@
     <col min="9" max="9" width="13.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16" width="14.28515625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="17" width="14.28515625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:17" ht="15.75">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:17">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:17">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+    <row r="4" spans="1:17">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+    <row r="5" spans="1:17">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="25.5">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="25.5">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="P6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -651,13 +662,14 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:P6"/>
+  <autoFilter ref="A6:Q6"/>
   <mergeCells count="3">
-    <mergeCell ref="A3:P5"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:Q5"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>